<commit_message>
finish rate algorithm demo
</commit_message>
<xml_diff>
--- a/apps/rate/rules/nginx-ops.xlsx
+++ b/apps/rate/rules/nginx-ops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k.song/src/dumpplane/apps/rate/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346955F-72D7-8349-A8AB-F6B0A5FB7CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3B3DD3-44FC-6340-BC91-329111EC1C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{29A2A310-46A5-1B4E-BFC5-6A69C9BFA7AA}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>worker_processes==$param</t>
   </si>
   <si>
-    <t>worker_connections==$param</t>
-  </si>
-  <si>
     <t>nginxfact.setResults($param);</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>nginxfact: NginxConfigDirectiveFact</t>
+  </si>
+  <si>
+    <t>worker_connections&lt;=$param</t>
   </si>
 </sst>
 </file>
@@ -222,26 +222,8 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -257,26 +239,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +595,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -926,44 +926,44 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="H3" s="11"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" s="11"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="H5" s="11"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -975,57 +975,57 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="13"/>
-      <c r="H7" s="11"/>
+      <c r="B7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="7"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="17" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1024</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="20">
-        <v>1024</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>